<commit_message>
feat(export): add dashboard PDF export functionality and refactor statistics formatting
- Implement new DashboardPdfService for generating PDF reports
- Add support for puskesmas-specific filtering in exports
- Refactor statistics formatting to match AdminAllFormatter standards
- Remove old PDF templates and replace with consolidated dashboard view
- Update ExportService to handle new dashboard export logic
</commit_message>
<xml_diff>
--- a/resources/templates/puskesmas.xlsx
+++ b/resources/templates/puskesmas.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Program\GitHub\akudihatinya\akudihatinya-backend\resources\views\exports\formatLaporanAkudihatinya\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Program\GitHub\akudihatinya\akudihatinya-backend\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E4DB78F-98D5-4B42-ADDD-59C766006AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE89127A-56F2-4AC8-8AB5-E3158E20C6C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{54DF6366-42DF-47E1-8A5D-3CF0032E5F84}"/>
   </bookViews>
   <sheets>
-    <sheet name="DM" sheetId="1" r:id="rId1"/>
+    <sheet name="&lt;Laporan&gt;" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>SASARAN</t>
   </si>
@@ -108,9 +108,6 @@
     <t>REKAPITULASI CAPAIAN STANDAR PELAYANAN MINIMAL  BIDANG KESEHATAN</t>
   </si>
   <si>
-    <t>TOTAL CAPAIAN TAHUN 2024</t>
-  </si>
-  <si>
     <t>L</t>
   </si>
   <si>
@@ -127,16 +124,26 @@
   </si>
   <si>
     <t>PUSKESMAS</t>
+  </si>
+  <si>
+    <t>&lt;sasaran&gt;</t>
+  </si>
+  <si>
+    <t>&lt;puskesmas&gt;</t>
+  </si>
+  <si>
+    <t>TOTAL CAPAIAN TAHUN &lt;tahun&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="#,##0.##"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00%"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -321,7 +328,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -361,41 +368,10 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -508,7 +484,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyBorder="0"/>
-    <xf numFmtId="166" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyBorder="0"/>
@@ -519,7 +495,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -528,18 +504,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -549,60 +513,93 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -965,13 +962,13 @@
   <dimension ref="A1:BQ25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="24.21875" customWidth="1"/>
-    <col min="2" max="6" width="7.21875" style="10" customWidth="1"/>
+    <col min="2" max="6" width="7.21875" style="6" customWidth="1"/>
     <col min="7" max="10" width="7.21875" customWidth="1"/>
     <col min="11" max="11" width="11.77734375" customWidth="1"/>
     <col min="12" max="12" width="12.21875" customWidth="1"/>
@@ -979,497 +976,588 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:69" s="1" customFormat="1" ht="21">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
-      <c r="Z1" s="34"/>
-      <c r="AA1" s="34"/>
-      <c r="AB1" s="34"/>
-      <c r="AC1" s="34"/>
-      <c r="AD1" s="34"/>
-      <c r="AE1" s="34"/>
-      <c r="AF1" s="34"/>
-      <c r="AG1" s="34"/>
-      <c r="AH1" s="34"/>
-      <c r="AI1" s="34"/>
-      <c r="AJ1" s="34"/>
-      <c r="AK1" s="34"/>
-      <c r="AL1" s="34"/>
-      <c r="AM1" s="34"/>
-      <c r="AN1" s="34"/>
-      <c r="AO1" s="34"/>
-      <c r="AP1" s="34"/>
-      <c r="AQ1" s="34"/>
-      <c r="AR1" s="34"/>
-      <c r="AS1" s="34"/>
-      <c r="AT1" s="34"/>
-      <c r="AU1" s="34"/>
-      <c r="AV1" s="34"/>
-      <c r="AW1" s="34"/>
-      <c r="AX1" s="34"/>
-      <c r="AY1" s="34"/>
-      <c r="AZ1" s="34"/>
-      <c r="BA1" s="34"/>
-      <c r="BB1" s="34"/>
-      <c r="BC1" s="34"/>
-      <c r="BD1" s="34"/>
-      <c r="BE1" s="34"/>
-      <c r="BF1" s="34"/>
-      <c r="BG1" s="34"/>
-      <c r="BH1" s="34"/>
-      <c r="BI1" s="34"/>
-      <c r="BJ1" s="34"/>
-      <c r="BK1" s="34"/>
-      <c r="BL1" s="34"/>
-      <c r="BM1" s="34"/>
-      <c r="BN1" s="34"/>
-      <c r="BO1" s="34"/>
-      <c r="BP1" s="34"/>
-      <c r="BQ1" s="34"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12"/>
+      <c r="AL1" s="12"/>
+      <c r="AM1" s="12"/>
+      <c r="AN1" s="12"/>
+      <c r="AO1" s="12"/>
+      <c r="AP1" s="12"/>
+      <c r="AQ1" s="12"/>
+      <c r="AR1" s="12"/>
+      <c r="AS1" s="12"/>
+      <c r="AT1" s="12"/>
+      <c r="AU1" s="12"/>
+      <c r="AV1" s="12"/>
+      <c r="AW1" s="12"/>
+      <c r="AX1" s="12"/>
+      <c r="AY1" s="12"/>
+      <c r="AZ1" s="12"/>
+      <c r="BA1" s="12"/>
+      <c r="BB1" s="12"/>
+      <c r="BC1" s="12"/>
+      <c r="BD1" s="12"/>
+      <c r="BE1" s="12"/>
+      <c r="BF1" s="12"/>
+      <c r="BG1" s="12"/>
+      <c r="BH1" s="12"/>
+      <c r="BI1" s="12"/>
+      <c r="BJ1" s="12"/>
+      <c r="BK1" s="12"/>
+      <c r="BL1" s="12"/>
+      <c r="BM1" s="12"/>
+      <c r="BN1" s="12"/>
+      <c r="BO1" s="12"/>
+      <c r="BP1" s="12"/>
+      <c r="BQ1" s="12"/>
     </row>
     <row r="2" spans="1:69" s="1" customFormat="1" ht="21">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="12"/>
+      <c r="AA2" s="12"/>
+      <c r="AB2" s="12"/>
+      <c r="AC2" s="12"/>
+      <c r="AD2" s="12"/>
+      <c r="AE2" s="12"/>
+      <c r="AF2" s="12"/>
+      <c r="AG2" s="12"/>
+      <c r="AH2" s="12"/>
+      <c r="AI2" s="12"/>
+      <c r="AJ2" s="12"/>
+      <c r="AK2" s="12"/>
+      <c r="AL2" s="12"/>
+      <c r="AM2" s="12"/>
+      <c r="AN2" s="12"/>
+      <c r="AO2" s="12"/>
+      <c r="AP2" s="12"/>
+      <c r="AQ2" s="12"/>
+      <c r="AR2" s="12"/>
+      <c r="AS2" s="12"/>
+      <c r="AT2" s="12"/>
+      <c r="AU2" s="12"/>
+      <c r="AV2" s="12"/>
+      <c r="AW2" s="12"/>
+      <c r="AX2" s="12"/>
+      <c r="AY2" s="12"/>
+      <c r="AZ2" s="12"/>
+      <c r="BA2" s="12"/>
+      <c r="BB2" s="12"/>
+      <c r="BC2" s="12"/>
+      <c r="BD2" s="12"/>
+      <c r="BE2" s="12"/>
+      <c r="BF2" s="12"/>
+      <c r="BG2" s="12"/>
+      <c r="BH2" s="12"/>
+      <c r="BI2" s="12"/>
+      <c r="BJ2" s="12"/>
+      <c r="BK2" s="12"/>
+      <c r="BL2" s="12"/>
+      <c r="BM2" s="12"/>
+      <c r="BN2" s="12"/>
+      <c r="BO2" s="12"/>
+      <c r="BP2" s="12"/>
+      <c r="BQ2" s="12"/>
+    </row>
+    <row r="3" spans="1:69" s="1" customFormat="1" ht="21">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
+      <c r="AA3" s="10"/>
+      <c r="AB3" s="10"/>
+      <c r="AC3" s="10"/>
+      <c r="AD3" s="10"/>
+      <c r="AE3" s="10"/>
+      <c r="AF3" s="10"/>
+      <c r="AG3" s="10"/>
+      <c r="AH3" s="10"/>
+      <c r="AI3" s="10"/>
+      <c r="AJ3" s="10"/>
+      <c r="AK3" s="10"/>
+      <c r="AL3" s="10"/>
+      <c r="AM3" s="10"/>
+      <c r="AN3" s="10"/>
+      <c r="AO3" s="10"/>
+      <c r="AP3" s="10"/>
+      <c r="AQ3" s="10"/>
+      <c r="AR3" s="10"/>
+      <c r="AS3" s="10"/>
+      <c r="AT3" s="10"/>
+      <c r="AU3" s="10"/>
+      <c r="AV3" s="10"/>
+      <c r="AW3" s="10"/>
+      <c r="AX3" s="10"/>
+      <c r="AY3" s="10"/>
+      <c r="AZ3" s="10"/>
+      <c r="BA3" s="10"/>
+      <c r="BB3" s="10"/>
+      <c r="BC3" s="10"/>
+      <c r="BD3" s="10"/>
+      <c r="BE3" s="10"/>
+      <c r="BF3" s="10"/>
+      <c r="BG3" s="10"/>
+      <c r="BH3" s="10"/>
+      <c r="BI3" s="10"/>
+      <c r="BJ3" s="10"/>
+      <c r="BK3" s="10"/>
+      <c r="BL3" s="10"/>
+      <c r="BM3" s="10"/>
+      <c r="BN3" s="10"/>
+      <c r="BO3" s="10"/>
+      <c r="BP3" s="10"/>
+      <c r="BQ3" s="10"/>
+    </row>
+    <row r="4" spans="1:69" s="1" customFormat="1" ht="21">
+      <c r="A4" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+    </row>
+    <row r="5" spans="1:69" s="1" customFormat="1" ht="21">
+      <c r="A5" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="34"/>
-      <c r="V2" s="34"/>
-      <c r="W2" s="34"/>
-      <c r="X2" s="34"/>
-      <c r="Y2" s="34"/>
-      <c r="Z2" s="34"/>
-      <c r="AA2" s="34"/>
-      <c r="AB2" s="34"/>
-      <c r="AC2" s="34"/>
-      <c r="AD2" s="34"/>
-      <c r="AE2" s="34"/>
-      <c r="AF2" s="34"/>
-      <c r="AG2" s="34"/>
-      <c r="AH2" s="34"/>
-      <c r="AI2" s="34"/>
-      <c r="AJ2" s="34"/>
-      <c r="AK2" s="34"/>
-      <c r="AL2" s="34"/>
-      <c r="AM2" s="34"/>
-      <c r="AN2" s="34"/>
-      <c r="AO2" s="34"/>
-      <c r="AP2" s="34"/>
-      <c r="AQ2" s="34"/>
-      <c r="AR2" s="34"/>
-      <c r="AS2" s="34"/>
-      <c r="AT2" s="34"/>
-      <c r="AU2" s="34"/>
-      <c r="AV2" s="34"/>
-      <c r="AW2" s="34"/>
-      <c r="AX2" s="34"/>
-      <c r="AY2" s="34"/>
-      <c r="AZ2" s="34"/>
-      <c r="BA2" s="34"/>
-      <c r="BB2" s="34"/>
-      <c r="BC2" s="34"/>
-      <c r="BD2" s="34"/>
-      <c r="BE2" s="34"/>
-      <c r="BF2" s="34"/>
-      <c r="BG2" s="34"/>
-      <c r="BH2" s="34"/>
-      <c r="BI2" s="34"/>
-      <c r="BJ2" s="34"/>
-      <c r="BK2" s="34"/>
-      <c r="BL2" s="34"/>
-      <c r="BM2" s="34"/>
-      <c r="BN2" s="34"/>
-      <c r="BO2" s="34"/>
-      <c r="BP2" s="34"/>
-      <c r="BQ2" s="34"/>
-    </row>
-    <row r="3" spans="1:69" s="1" customFormat="1" ht="21">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14"/>
-      <c r="V3" s="14"/>
-      <c r="W3" s="14"/>
-      <c r="X3" s="14"/>
-      <c r="Y3" s="14"/>
-      <c r="Z3" s="14"/>
-      <c r="AA3" s="14"/>
-      <c r="AB3" s="14"/>
-      <c r="AC3" s="14"/>
-      <c r="AD3" s="14"/>
-      <c r="AE3" s="14"/>
-      <c r="AF3" s="14"/>
-      <c r="AG3" s="14"/>
-      <c r="AH3" s="14"/>
-      <c r="AI3" s="14"/>
-      <c r="AJ3" s="14"/>
-      <c r="AK3" s="14"/>
-      <c r="AL3" s="14"/>
-      <c r="AM3" s="14"/>
-      <c r="AN3" s="14"/>
-      <c r="AO3" s="14"/>
-      <c r="AP3" s="14"/>
-      <c r="AQ3" s="14"/>
-      <c r="AR3" s="14"/>
-      <c r="AS3" s="14"/>
-      <c r="AT3" s="14"/>
-      <c r="AU3" s="14"/>
-      <c r="AV3" s="14"/>
-      <c r="AW3" s="14"/>
-      <c r="AX3" s="14"/>
-      <c r="AY3" s="14"/>
-      <c r="AZ3" s="14"/>
-      <c r="BA3" s="14"/>
-      <c r="BB3" s="14"/>
-      <c r="BC3" s="14"/>
-      <c r="BD3" s="14"/>
-      <c r="BE3" s="14"/>
-      <c r="BF3" s="14"/>
-      <c r="BG3" s="14"/>
-      <c r="BH3" s="14"/>
-      <c r="BI3" s="14"/>
-      <c r="BJ3" s="14"/>
-      <c r="BK3" s="14"/>
-      <c r="BL3" s="14"/>
-      <c r="BM3" s="14"/>
-      <c r="BN3" s="14"/>
-      <c r="BO3" s="14"/>
-      <c r="BP3" s="14"/>
-      <c r="BQ3" s="14"/>
-    </row>
-    <row r="4" spans="1:69" s="1" customFormat="1" ht="21">
-      <c r="A4" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-    </row>
-    <row r="5" spans="1:69" s="1" customFormat="1" ht="21">
-      <c r="A5" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
+      <c r="B5" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
     </row>
     <row r="7" spans="1:69" s="3" customFormat="1" ht="21.6" customHeight="1">
-      <c r="A7" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="20" t="s">
+      <c r="A7" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="21" t="s">
+      <c r="C7" s="38"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="F7" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="M7" s="32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:69" s="3" customFormat="1" ht="21.6" customHeight="1">
+      <c r="A8" s="36"/>
+      <c r="B8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="M7" s="25" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:69" s="3" customFormat="1" ht="21.6" customHeight="1">
-      <c r="A8" s="24"/>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="H8" s="20" t="s">
+      <c r="E8" s="29"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="18"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="21" t="s">
+      <c r="I8" s="38"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-    </row>
-    <row r="9" spans="1:69" s="13" customFormat="1" ht="15" customHeight="1">
-      <c r="A9" s="11" t="s">
+      <c r="L8" s="33"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="9"/>
+    </row>
+    <row r="9" spans="1:69" s="9" customFormat="1" ht="15" customHeight="1">
+      <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="H9" s="2" t="s">
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="15"/>
+      <c r="H9" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="22"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="27"/>
-    </row>
-    <row r="10" spans="1:69" s="13" customFormat="1" ht="15" customHeight="1">
-      <c r="A10" s="11" t="s">
+      <c r="K9" s="29"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+    </row>
+    <row r="10" spans="1:69" s="9" customFormat="1" ht="15" customHeight="1">
+      <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="31"/>
-    </row>
-    <row r="11" spans="1:69" s="13" customFormat="1" ht="15" customHeight="1">
-      <c r="A11" s="11" t="s">
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="15"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="24"/>
+    </row>
+    <row r="11" spans="1:69" s="9" customFormat="1" ht="15" customHeight="1">
+      <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:69" s="13" customFormat="1" ht="15" customHeight="1">
-      <c r="A12" s="32" t="s">
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="15"/>
+    </row>
+    <row r="12" spans="1:69" s="9" customFormat="1" ht="15" customHeight="1">
+      <c r="A12" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-    </row>
-    <row r="13" spans="1:69" s="13" customFormat="1" ht="15" customHeight="1">
-      <c r="A13" s="11" t="s">
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="24"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+    </row>
+    <row r="13" spans="1:69" s="9" customFormat="1" ht="15" customHeight="1">
+      <c r="A13" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:69" s="12" customFormat="1">
-      <c r="A14" s="11" t="s">
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+    </row>
+    <row r="14" spans="1:69" s="8" customFormat="1" ht="15.6">
+      <c r="A14" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-    </row>
-    <row r="15" spans="1:69" s="12" customFormat="1">
-      <c r="A15" s="11" t="s">
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="18"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+    </row>
+    <row r="15" spans="1:69" s="8" customFormat="1" ht="15.6">
+      <c r="A15" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-    </row>
-    <row r="16" spans="1:69" s="13" customFormat="1" ht="15" customHeight="1">
-      <c r="A16" s="32" t="s">
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="9"/>
+      <c r="N15" s="9"/>
+    </row>
+    <row r="16" spans="1:69" s="9" customFormat="1" ht="15" customHeight="1">
+      <c r="A16" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-    </row>
-    <row r="17" spans="1:6" s="12" customFormat="1">
-      <c r="A17" s="11" t="s">
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+    </row>
+    <row r="17" spans="1:14" s="8" customFormat="1">
+      <c r="A17" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-    </row>
-    <row r="18" spans="1:6" s="12" customFormat="1">
-      <c r="A18" s="11" t="s">
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="18"/>
+    </row>
+    <row r="18" spans="1:14" s="8" customFormat="1" ht="15.6">
+      <c r="A18" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-    </row>
-    <row r="19" spans="1:6" s="12" customFormat="1">
-      <c r="A19" s="11" t="s">
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="18"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+    </row>
+    <row r="19" spans="1:14" s="8" customFormat="1" ht="15.6">
+      <c r="A19" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-    </row>
-    <row r="20" spans="1:6" s="13" customFormat="1" ht="15" customHeight="1">
-      <c r="A20" s="32" t="s">
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="9"/>
+      <c r="N19" s="9"/>
+    </row>
+    <row r="20" spans="1:14" s="9" customFormat="1" ht="15" customHeight="1">
+      <c r="A20" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-    </row>
-    <row r="21" spans="1:6" s="12" customFormat="1">
-      <c r="A21" s="11" t="s">
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="8"/>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20" s="8"/>
+    </row>
+    <row r="21" spans="1:14" s="8" customFormat="1">
+      <c r="A21" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="20"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="N21"/>
+    </row>
+    <row r="22" spans="1:14" ht="15.6">
       <c r="A22" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="20"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+    </row>
+    <row r="23" spans="1:14" ht="15.6">
       <c r="A23" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-    </row>
-    <row r="24" spans="1:6" s="13" customFormat="1" ht="15" customHeight="1">
-      <c r="A24" s="32" t="s">
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="9"/>
+      <c r="N23" s="9"/>
+    </row>
+    <row r="24" spans="1:14" s="9" customFormat="1" ht="15" customHeight="1">
+      <c r="A24" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="26"/>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24"/>
+      <c r="M24"/>
+      <c r="N24"/>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
+      <c r="B25" s="21">
+        <f>SUM(B9:B24)</f>
+        <v>0</v>
+      </c>
+      <c r="C25" s="21">
+        <f t="shared" ref="C25:E25" si="0">SUM(C9:C24)</f>
+        <v>0</v>
+      </c>
+      <c r="D25" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E25" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="22">
+        <f>SUM(F9:F24)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>